<commit_message>
adding SQLalchemy DB read
</commit_message>
<xml_diff>
--- a/db_sample_101119.xlsx
+++ b/db_sample_101119.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skawashi/PycharmProjects/dbtest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203EE894-BBC4-EF42-9141-703256F4C08B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120F7E46-002A-3F47-9CB4-0AF3DD50EEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57300" yWindow="1120" windowWidth="26560" windowHeight="15640" xr2:uid="{789105E0-E448-F34E-B909-65F8D414E133}"/>
+    <workbookView xWindow="57460" yWindow="2940" windowWidth="26560" windowHeight="15640" xr2:uid="{789105E0-E448-F34E-B909-65F8D414E133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,48 +31,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="43">
-  <si>
-    <t>2019-10-11-151335</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="44">
   <si>
     <t>Tsunami</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2019-10-11-151200</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2019-10-11-162342</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Typhoon</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2019-10-11-162200</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2019-10-11-173312</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Earthquake</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2019-10-11-173200</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2019-10-09-100008</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Flood</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -201,6 +173,38 @@
   </si>
   <si>
     <t>typhoon_speed  INTEGER</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019-15:12</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019-17:32</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019-16:22</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019 17:32</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019  15:13</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019  17:33</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11 OCT 2019  16:23</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>09 OCT 2019  10:00</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -254,11 +258,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -578,7 +585,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -595,16 +602,16 @@
     <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="22.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="2" customWidth="1"/>
     <col min="14" max="14" width="19" style="1" customWidth="1"/>
     <col min="15" max="15" width="21.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="1" customWidth="1"/>
     <col min="17" max="17" width="16.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="21.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" style="2" customWidth="1"/>
     <col min="20" max="20" width="23.5703125" style="1" customWidth="1"/>
     <col min="21" max="21" width="23.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="18" style="1" customWidth="1"/>
+    <col min="22" max="22" width="18" style="2" customWidth="1"/>
     <col min="23" max="23" width="21.42578125" style="1" customWidth="1"/>
     <col min="24" max="24" width="27.140625" style="1" customWidth="1"/>
     <col min="25" max="28" width="26.5703125" style="1" customWidth="1"/>
@@ -613,94 +620,94 @@
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="B2" s="1">
         <v>35.606453199999997</v>
       </c>
@@ -708,7 +715,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
@@ -734,22 +741,22 @@
       <c r="L2" s="1">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>2</v>
+      <c r="M2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>8</v>
+      <c r="S2" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
+      <c r="A3" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="1">
         <v>35.606453199999997</v>
@@ -758,7 +765,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -784,22 +791,22 @@
       <c r="L3" s="1">
         <v>13</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>2</v>
+      <c r="M3" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R3" s="1">
         <v>1</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>8</v>
+      <c r="S3" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
+      <c r="A4" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="1">
         <v>35.606453199999997</v>
@@ -808,7 +815,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -834,22 +841,22 @@
       <c r="L4" s="1">
         <v>13</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>2</v>
+      <c r="M4" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R4" s="1">
         <v>3</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>8</v>
+      <c r="S4" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
+      <c r="A5" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B5" s="1">
         <v>35.606453199999997</v>
@@ -858,7 +865,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -884,22 +891,22 @@
       <c r="L5" s="1">
         <v>13</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>2</v>
+      <c r="M5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R5" s="1">
         <v>3</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>8</v>
+      <c r="S5" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>35.606453199999997</v>
@@ -908,7 +915,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -934,11 +941,11 @@
       <c r="L6" s="1">
         <v>0</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>8</v>
+      <c r="M6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O6" s="1">
         <v>35.397325799999997</v>
@@ -951,8 +958,8 @@
       </c>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+      <c r="A7" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="1">
         <v>35.606453199999997</v>
@@ -961,7 +968,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -987,11 +994,11 @@
       <c r="L7" s="1">
         <v>0</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>8</v>
+      <c r="M7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O7" s="1">
         <v>35.397325799999997</v>
@@ -1004,8 +1011,8 @@
       </c>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
+      <c r="A8" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B8" s="1">
         <v>35.606453199999997</v>
@@ -1014,7 +1021,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -1040,11 +1047,11 @@
       <c r="L8" s="1">
         <v>0</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>8</v>
+      <c r="M8" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O8" s="1">
         <v>35.397325799999997</v>
@@ -1057,8 +1064,8 @@
       </c>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
+      <c r="A9" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>35.606453199999997</v>
@@ -1067,7 +1074,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
@@ -1093,11 +1100,11 @@
       <c r="L9" s="1">
         <v>0</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>8</v>
+      <c r="M9" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O9" s="1">
         <v>35.397325799999997</v>
@@ -1110,8 +1117,8 @@
       </c>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
+      <c r="A10" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B10" s="1">
         <v>35.606453199999997</v>
@@ -1120,7 +1127,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
@@ -1146,11 +1153,11 @@
       <c r="L10" s="1">
         <v>0</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>8</v>
+      <c r="M10" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O10" s="1">
         <v>35.397325799999997</v>
@@ -1163,8 +1170,8 @@
       </c>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
+      <c r="A11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B11" s="1">
         <v>35.606453199999997</v>
@@ -1173,7 +1180,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
@@ -1199,11 +1206,11 @@
       <c r="L11" s="1">
         <v>0</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>8</v>
+      <c r="M11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="O11" s="1">
         <v>35.397325799999997</v>
@@ -1216,8 +1223,8 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="21" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
+      <c r="A12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="1">
         <v>35.606453199999997</v>
@@ -1226,7 +1233,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1252,11 +1259,11 @@
       <c r="L12" s="1">
         <v>65</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>5</v>
+      <c r="M12" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T12" s="1">
         <v>33.076563999999998</v>
@@ -1264,11 +1271,11 @@
       <c r="U12" s="1">
         <v>139.05918800000001</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>8</v>
+      <c r="V12" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="X12" s="1">
         <v>50</v>
@@ -1280,15 +1287,15 @@
         <v>999</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AB12" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="21" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
+      <c r="A13" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="1">
         <v>35.606453199999997</v>
@@ -1297,7 +1304,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1323,11 +1330,11 @@
       <c r="L13" s="1">
         <v>65</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>5</v>
+      <c r="M13" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T13" s="1">
         <v>33.076563999999998</v>
@@ -1335,11 +1342,11 @@
       <c r="U13" s="1">
         <v>139.05918800000001</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>8</v>
+      <c r="V13" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="X13" s="1">
         <v>50</v>
@@ -1351,15 +1358,15 @@
         <v>999</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AB13" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="21" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>3</v>
+      <c r="A14" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B14" s="1">
         <v>35.606453199999997</v>
@@ -1368,7 +1375,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1394,11 +1401,11 @@
       <c r="L14" s="1">
         <v>65</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>5</v>
+      <c r="M14" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T14" s="1">
         <v>33.076563999999998</v>
@@ -1406,11 +1413,11 @@
       <c r="U14" s="1">
         <v>139.05918800000001</v>
       </c>
-      <c r="V14" s="1" t="s">
-        <v>8</v>
+      <c r="V14" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="X14" s="1">
         <v>115</v>
@@ -1422,15 +1429,15 @@
         <v>950</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AB14" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="21" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
+      <c r="A15" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B15" s="1">
         <v>35.606453199999997</v>
@@ -1439,7 +1446,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1465,11 +1472,11 @@
       <c r="L15" s="1">
         <v>65</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>5</v>
+      <c r="M15" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T15" s="1">
         <v>33.076563999999998</v>
@@ -1477,11 +1484,11 @@
       <c r="U15" s="1">
         <v>139.05918800000001</v>
       </c>
-      <c r="V15" s="1" t="s">
-        <v>8</v>
+      <c r="V15" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="X15" s="1">
         <v>115</v>
@@ -1493,15 +1500,15 @@
         <v>950</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AB15" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="21" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
+      <c r="A16" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B16" s="1">
         <v>35.606453199999997</v>
@@ -1510,7 +1517,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
@@ -1536,11 +1543,11 @@
       <c r="L16" s="1">
         <v>65</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>5</v>
+      <c r="M16" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T16" s="1">
         <v>35.657857200000002</v>
@@ -1548,11 +1555,11 @@
       <c r="U16" s="1">
         <v>139.82045110000001</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>8</v>
+      <c r="V16" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="X16" s="1">
         <v>115</v>
@@ -1564,15 +1571,15 @@
         <v>950</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AB16" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="21" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
+      <c r="A17" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B17" s="1">
         <v>35.606453199999997</v>
@@ -1581,7 +1588,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
         <v>4</v>
@@ -1607,11 +1614,11 @@
       <c r="L17" s="1">
         <v>65</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>5</v>
+      <c r="M17" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T17" s="1">
         <v>35.657857200000002</v>
@@ -1619,11 +1626,11 @@
       <c r="U17" s="1">
         <v>139.82045110000001</v>
       </c>
-      <c r="V17" s="1" t="s">
-        <v>8</v>
+      <c r="V17" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="X17" s="1">
         <v>115</v>
@@ -1635,15 +1642,15 @@
         <v>950</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AB17" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="21" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
+      <c r="A18" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B18" s="1">
         <v>35.606453199999997</v>
@@ -1652,7 +1659,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -1678,16 +1685,16 @@
       <c r="L18" s="1">
         <v>-46</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>8</v>
+      <c r="M18" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="21" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>9</v>
+      <c r="A19" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B19" s="1">
         <v>35.606453199999997</v>
@@ -1696,7 +1703,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -1722,16 +1729,16 @@
       <c r="L19" s="1">
         <v>-46</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>8</v>
+      <c r="M19" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="21" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
+      <c r="A20" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B20" s="1">
         <v>35.606453199999997</v>
@@ -1740,7 +1747,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
@@ -1766,16 +1773,16 @@
       <c r="L20" s="1">
         <v>-46</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>8</v>
+      <c r="M20" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="21" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
+      <c r="A21" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B21" s="1">
         <v>35.606453199999997</v>
@@ -1784,7 +1791,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -1810,16 +1817,16 @@
       <c r="L21" s="1">
         <v>-46</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>8</v>
+      <c r="M21" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="21" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
+      <c r="A22" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B22" s="1">
         <v>35.606453199999997</v>
@@ -1828,7 +1835,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -1854,16 +1861,16 @@
       <c r="L22" s="1">
         <v>-46</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>8</v>
+      <c r="M22" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="21" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
+      <c r="A23" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B23" s="1">
         <v>35.606453199999997</v>
@@ -1872,7 +1879,7 @@
         <v>139.74914609999999</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1">
         <v>4</v>
@@ -1898,11 +1905,11 @@
       <c r="L23" s="1">
         <v>-46</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>8</v>
+      <c r="M23" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>